<commit_message>
chore: update data/source.xlsx and source.parquet from Drive
</commit_message>
<xml_diff>
--- a/data/source.xlsx
+++ b/data/source.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofstandrews907-my.sharepoint.com/personal/wrlc_st-andrews_ac_uk/Documents/Biodiversity at St Andrews/Biodiversity Action Plan/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://universityofstandrews907-my.sharepoint.com/personal/wrlc_st-andrews_ac_uk/Documents/Biodiversity at St Andrews/Biodiversity Action Plan/Biodiversity Action Plan Dashboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="14_{E0462596-C42A-4E25-8CC3-6C893004039D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="100" documentId="14_{E0462596-C42A-4E25-8CC3-6C893004039D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1962A733-4D6C-4D60-9F1A-A96926268758}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2105" uniqueCount="432">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2120" uniqueCount="469">
   <si>
     <t>Status</t>
   </si>
@@ -1773,12 +1773,136 @@
   <si>
     <t>Timescale</t>
   </si>
+  <si>
+    <t>Remove invasive animals throughout the Estates</t>
+  </si>
+  <si>
+    <t>M = Repeated surveys and adhoc sightings
+NOTE. No University action planned for grey squirrels at this time because of reputational, ethical and practical considerations</t>
+  </si>
+  <si>
+    <t>M = Habitat area monitoring 
+NOTE Progressing at the individual site level through habitat area plans</t>
+  </si>
+  <si>
+    <t>M = Creation of repository
+NOTE: In planning stage with partnership of Botanic Garden</t>
+  </si>
+  <si>
+    <t>Harry Watkins, John Reid</t>
+  </si>
+  <si>
+    <t>S = Manage waterway vegetation by leaving a min. 2m of bankside vegetation, cut alternative banks each year, and trim vegetation late in summer to reduce disturbance during breeding season (late September/October)
+M =Habitat area and biodiversity monitoring
+A = inexpensive; change in management recommendations
+R = many species require bankside cover
+T = Not currently manage any waterways</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S = Plant mixed species stands of woodland (coniferous and deciduous)
+M = No. trees planted and established; habitat area monitoring
+</t>
+  </si>
+  <si>
+    <t>Retain and encourage ivy on trees  and raise awareness about value and myths through toolbox talk</t>
+  </si>
+  <si>
+    <t>M = Habitat area and biodiversity monitoring</t>
+  </si>
+  <si>
+    <t>M = Biodiversity monitoring</t>
+  </si>
+  <si>
+    <t>M = Habitat infrastructure and biodiversity monitoring</t>
+  </si>
+  <si>
+    <t>M = Biodiversity monitoring and dashboard</t>
+  </si>
+  <si>
+    <t>M = Habitat area monitoring</t>
+  </si>
+  <si>
+    <t>Development planning project teams and Biodiversity Working Group</t>
+  </si>
+  <si>
+    <t>Keith Thomason and Will Cresswell</t>
+  </si>
+  <si>
+    <t>Harry Watkins, John Reid, Will Cresswell</t>
+  </si>
+  <si>
+    <t>Botanic Gardens and Estates</t>
+  </si>
+  <si>
+    <t>M = Biodiversity Working Group logs involvement in development projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M = Measured by number of people visiting museum and feedback forms at the museum
+</t>
+  </si>
+  <si>
+    <t>M = no. of meetings, no. of collaborative projects</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M = Volume of research conducted at undergraduate and postgraduate level
+</t>
+  </si>
+  <si>
+    <t>University Sustainability in the Curriculum person when this appears</t>
+  </si>
+  <si>
+    <t>M = Garden created, research underway
+NOTE: Garden adjacent to St Mary's Quad/Bute Building is being developed as a wild garden with some sensory features</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M = Before and after questionnaires; number of students involved in biodiversity projects
+</t>
+  </si>
+  <si>
+    <t>Biodiversity Literacy Module</t>
+  </si>
+  <si>
+    <t>Amanda Skinner</t>
+  </si>
+  <si>
+    <t>Sustainability Comms lead</t>
+  </si>
+  <si>
+    <t>Role created to create a pathway for students to get accreditation for sustainable modules and activities</t>
+  </si>
+  <si>
+    <t>University governance; Principal's Office</t>
+  </si>
+  <si>
+    <t>M = Occurrence of Sustainability Summit annually</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Embracing the sustainability summit </t>
+  </si>
+  <si>
+    <t>More formal and frequent communications from senior leadership</t>
+  </si>
+  <si>
+    <t>Official role responsible for biodiversity positive in development  projects</t>
+  </si>
+  <si>
+    <t>Biodiversity expertise a priority in staff hires in grounds</t>
+  </si>
+  <si>
+    <t>Karen Laing</t>
+  </si>
+  <si>
+    <t>Ecological Projects Officer; University governance; Principal's Office</t>
+  </si>
+  <si>
+    <t>Senior leadership group has a biodiversity champion</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1939,6 +2063,14 @@
     <font>
       <b/>
       <sz val="15"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -2280,7 +2412,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="200">
+  <cellXfs count="201">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -2818,7 +2950,10 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="23" fillId="14" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="13" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2827,7 +2962,28 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="12">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC00000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor theme="9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <fill>
         <patternFill>
@@ -3201,13 +3357,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9F2F7B6-167F-48F0-8E37-93061261A30C}">
-  <dimension ref="A1:W66"/>
+  <dimension ref="A1:W64"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="2" topLeftCell="C58" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="2" topLeftCell="C3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="A3" sqref="A3:A66"/>
+      <selection pane="bottomRight" activeCell="F60" sqref="F60:F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -3817,18 +3973,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:22" ht="255">
+    <row r="15" spans="1:22" ht="76.5">
       <c r="A15" s="10" t="s">
         <v>124</v>
       </c>
       <c r="B15" s="126" t="s">
-        <v>125</v>
+        <v>432</v>
       </c>
       <c r="C15" s="117" t="s">
         <v>126</v>
       </c>
       <c r="D15" s="169" t="s">
-        <v>127</v>
+        <v>433</v>
       </c>
       <c r="E15" s="170" t="s">
         <v>128</v>
@@ -3889,9 +4045,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:23" ht="127.5">
+    <row r="17" spans="1:23" ht="45">
       <c r="A17" s="10" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B17" s="117" t="s">
         <v>145</v>
@@ -3900,7 +4056,7 @@
         <v>126</v>
       </c>
       <c r="D17" s="169" t="s">
-        <v>146</v>
+        <v>434</v>
       </c>
       <c r="E17" s="170"/>
       <c r="F17" s="117" t="s">
@@ -3925,9 +4081,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:23" ht="89.25">
+    <row r="18" spans="1:23" ht="38.25">
       <c r="A18" s="10" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B18" s="117" t="s">
         <v>150</v>
@@ -3936,10 +4092,10 @@
         <v>151</v>
       </c>
       <c r="D18" s="169" t="s">
-        <v>152</v>
+        <v>435</v>
       </c>
       <c r="E18" s="170" t="s">
-        <v>19</v>
+        <v>436</v>
       </c>
       <c r="F18" s="117" t="s">
         <v>50</v>
@@ -3965,7 +4121,7 @@
     </row>
     <row r="19" spans="1:23" ht="153">
       <c r="A19" s="10" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B19" s="117" t="s">
         <v>156</v>
@@ -3974,10 +4130,10 @@
         <v>157</v>
       </c>
       <c r="D19" s="169" t="s">
-        <v>158</v>
+        <v>437</v>
       </c>
       <c r="E19" s="170" t="s">
-        <v>119</v>
+        <v>19</v>
       </c>
       <c r="F19" s="117" t="s">
         <v>159</v>
@@ -4046,9 +4202,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:23" ht="191.25">
+    <row r="21" spans="1:23" ht="75">
       <c r="A21" s="10" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B21" s="117" t="s">
         <v>171</v>
@@ -4057,7 +4213,7 @@
         <v>172</v>
       </c>
       <c r="D21" s="169" t="s">
-        <v>173</v>
+        <v>438</v>
       </c>
       <c r="E21" s="170" t="s">
         <v>16</v>
@@ -4102,18 +4258,18 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:23" ht="114.75">
+    <row r="22" spans="1:23" ht="75">
       <c r="A22" s="76" t="s">
         <v>124</v>
       </c>
       <c r="B22" s="126" t="s">
-        <v>176</v>
+        <v>439</v>
       </c>
       <c r="C22" s="117" t="s">
         <v>177</v>
       </c>
       <c r="D22" s="169" t="s">
-        <v>178</v>
+        <v>440</v>
       </c>
       <c r="E22" s="170" t="s">
         <v>19</v>
@@ -4146,9 +4302,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:23" ht="140.25">
+    <row r="23" spans="1:23" ht="75">
       <c r="A23" s="173" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B23" s="117" t="s">
         <v>182</v>
@@ -4157,13 +4313,13 @@
         <v>126</v>
       </c>
       <c r="D23" s="169" t="s">
-        <v>183</v>
+        <v>441</v>
       </c>
       <c r="E23" s="170" t="s">
         <v>119</v>
       </c>
       <c r="F23" s="117" t="s">
-        <v>170</v>
+        <v>246</v>
       </c>
       <c r="G23" s="117" t="s">
         <v>27</v>
@@ -4546,7 +4702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:22" ht="318.75">
+    <row r="33" spans="1:22" ht="120">
       <c r="A33" s="10" t="s">
         <v>135</v>
       </c>
@@ -4557,7 +4713,7 @@
         <v>126</v>
       </c>
       <c r="D33" s="169" t="s">
-        <v>249</v>
+        <v>442</v>
       </c>
       <c r="E33" s="170" t="s">
         <v>250</v>
@@ -4584,7 +4740,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:22" ht="140.25">
+    <row r="34" spans="1:22" ht="75">
       <c r="A34" s="10" t="s">
         <v>21</v>
       </c>
@@ -4595,7 +4751,7 @@
         <v>257</v>
       </c>
       <c r="D34" s="169" t="s">
-        <v>258</v>
+        <v>443</v>
       </c>
       <c r="E34" s="170" t="s">
         <v>119</v>
@@ -4624,15 +4780,23 @@
     </row>
     <row r="35" spans="1:22" ht="75">
       <c r="A35" s="10" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B35" s="126" t="s">
         <v>261</v>
       </c>
-      <c r="C35" s="126"/>
-      <c r="D35" s="126"/>
-      <c r="E35" s="126"/>
-      <c r="F35" s="126"/>
+      <c r="C35" s="126" t="s">
+        <v>126</v>
+      </c>
+      <c r="D35" s="126" t="s">
+        <v>444</v>
+      </c>
+      <c r="E35" s="199" t="s">
+        <v>446</v>
+      </c>
+      <c r="F35" s="126" t="s">
+        <v>445</v>
+      </c>
       <c r="G35" s="126" t="s">
         <v>27</v>
       </c>
@@ -4659,10 +4823,18 @@
       <c r="B36" s="126" t="s">
         <v>429</v>
       </c>
-      <c r="C36" s="126"/>
-      <c r="D36" s="126"/>
-      <c r="E36" s="126"/>
-      <c r="F36" s="126"/>
+      <c r="C36" s="126" t="s">
+        <v>126</v>
+      </c>
+      <c r="D36" s="126" t="s">
+        <v>441</v>
+      </c>
+      <c r="E36" s="199" t="s">
+        <v>447</v>
+      </c>
+      <c r="F36" s="126" t="s">
+        <v>448</v>
+      </c>
       <c r="G36" s="126" t="s">
         <v>27</v>
       </c>
@@ -4680,15 +4852,23 @@
     </row>
     <row r="37" spans="1:22" ht="75">
       <c r="A37" s="10" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B37" s="126" t="s">
         <v>270</v>
       </c>
-      <c r="C37" s="126"/>
-      <c r="D37" s="126"/>
-      <c r="E37" s="126"/>
-      <c r="F37" s="126"/>
+      <c r="C37" s="126" t="s">
+        <v>126</v>
+      </c>
+      <c r="D37" s="126" t="s">
+        <v>434</v>
+      </c>
+      <c r="E37" s="170" t="s">
+        <v>119</v>
+      </c>
+      <c r="F37" s="117" t="s">
+        <v>246</v>
+      </c>
       <c r="G37" s="126" t="s">
         <v>27</v>
       </c>
@@ -4704,7 +4884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:22" ht="180">
+    <row r="38" spans="1:22" ht="60">
       <c r="A38" s="18" t="s">
         <v>124</v>
       </c>
@@ -4715,10 +4895,10 @@
         <v>244</v>
       </c>
       <c r="D38" s="126" t="s">
-        <v>264</v>
-      </c>
-      <c r="E38" s="126" t="s">
-        <v>265</v>
+        <v>449</v>
+      </c>
+      <c r="E38" s="199" t="s">
+        <v>446</v>
       </c>
       <c r="F38" s="126" t="s">
         <v>266</v>
@@ -4738,9 +4918,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:22" ht="60">
+    <row r="39" spans="1:22" ht="75">
       <c r="A39" s="174" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B39" s="175" t="s">
         <v>272</v>
@@ -4748,9 +4928,15 @@
       <c r="C39" s="175" t="s">
         <v>244</v>
       </c>
-      <c r="D39" s="175"/>
-      <c r="E39" s="175"/>
-      <c r="F39" s="175"/>
+      <c r="D39" s="175" t="s">
+        <v>444</v>
+      </c>
+      <c r="E39" s="170" t="s">
+        <v>119</v>
+      </c>
+      <c r="F39" s="117" t="s">
+        <v>246</v>
+      </c>
       <c r="G39" s="175" t="s">
         <v>27</v>
       </c>
@@ -4922,9 +5108,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="44" spans="1:22" ht="153">
+    <row r="44" spans="1:22" ht="105">
       <c r="A44" s="89" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B44" s="89" t="s">
         <v>307</v>
@@ -4933,7 +5119,7 @@
         <v>308</v>
       </c>
       <c r="D44" s="182" t="s">
-        <v>309</v>
+        <v>450</v>
       </c>
       <c r="E44" s="183" t="s">
         <v>310</v>
@@ -4960,7 +5146,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="45" spans="1:22" ht="153">
+    <row r="45" spans="1:22" ht="60">
       <c r="A45" s="89" t="s">
         <v>21</v>
       </c>
@@ -4971,7 +5157,7 @@
         <v>315</v>
       </c>
       <c r="D45" s="182" t="s">
-        <v>316</v>
+        <v>451</v>
       </c>
       <c r="E45" s="183" t="s">
         <v>139</v>
@@ -4998,7 +5184,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:22" ht="229.5">
+    <row r="46" spans="1:22" ht="60">
       <c r="A46" s="89" t="s">
         <v>124</v>
       </c>
@@ -5009,10 +5195,10 @@
         <v>321</v>
       </c>
       <c r="D46" s="182" t="s">
-        <v>322</v>
+        <v>452</v>
       </c>
       <c r="E46" s="183" t="s">
-        <v>139</v>
+        <v>453</v>
       </c>
       <c r="F46" s="89" t="s">
         <v>323</v>
@@ -5034,9 +5220,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:22" ht="191.25">
+    <row r="47" spans="1:22" ht="75">
       <c r="A47" s="89" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B47" s="88" t="s">
         <v>326</v>
@@ -5045,10 +5231,10 @@
         <v>327</v>
       </c>
       <c r="D47" s="182" t="s">
-        <v>328</v>
+        <v>454</v>
       </c>
       <c r="E47" s="183" t="s">
-        <v>119</v>
+        <v>19</v>
       </c>
       <c r="F47" s="89" t="s">
         <v>329</v>
@@ -5162,10 +5348,10 @@
         <v>346</v>
       </c>
       <c r="E50" s="183" t="s">
-        <v>347</v>
+        <v>119</v>
       </c>
       <c r="F50" s="89" t="s">
-        <v>348</v>
+        <v>119</v>
       </c>
       <c r="G50" s="89" t="s">
         <v>282</v>
@@ -5186,9 +5372,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:12" ht="114.75">
+    <row r="51" spans="1:12" ht="51">
       <c r="A51" s="89" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B51" s="103" t="s">
         <v>353</v>
@@ -5197,11 +5383,13 @@
         <v>354</v>
       </c>
       <c r="D51" s="182" t="s">
-        <v>355</v>
-      </c>
-      <c r="E51" s="183"/>
+        <v>455</v>
+      </c>
+      <c r="E51" s="183" t="s">
+        <v>119</v>
+      </c>
       <c r="F51" s="89" t="s">
-        <v>356</v>
+        <v>456</v>
       </c>
       <c r="G51" s="89" t="s">
         <v>282</v>
@@ -5222,24 +5410,24 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:12" ht="127.5">
+    <row r="52" spans="1:12" ht="153">
       <c r="A52" s="89" t="s">
-        <v>124</v>
+        <v>135</v>
       </c>
       <c r="B52" s="89" t="s">
-        <v>360</v>
+        <v>366</v>
       </c>
       <c r="C52" s="89" t="s">
-        <v>361</v>
+        <v>367</v>
       </c>
       <c r="D52" s="182" t="s">
-        <v>362</v>
+        <v>368</v>
       </c>
       <c r="E52" s="183" t="s">
         <v>119</v>
       </c>
       <c r="F52" s="89" t="s">
-        <v>313</v>
+        <v>246</v>
       </c>
       <c r="G52" s="89" t="s">
         <v>282</v>
@@ -5248,7 +5436,7 @@
         <v>43</v>
       </c>
       <c r="I52" s="180" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J52" s="180" t="s">
         <v>46</v>
@@ -5260,105 +5448,105 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:12" ht="153">
+    <row r="53" spans="1:12" ht="280.5">
       <c r="A53" s="89" t="s">
         <v>135</v>
       </c>
       <c r="B53" s="89" t="s">
-        <v>366</v>
+        <v>371</v>
       </c>
       <c r="C53" s="89" t="s">
-        <v>367</v>
+        <v>372</v>
       </c>
       <c r="D53" s="182" t="s">
-        <v>368</v>
+        <v>373</v>
       </c>
       <c r="E53" s="183" t="s">
         <v>119</v>
       </c>
-      <c r="F53" s="89" t="s">
-        <v>246</v>
+      <c r="F53" s="182" t="s">
+        <v>453</v>
       </c>
       <c r="G53" s="89" t="s">
         <v>282</v>
       </c>
       <c r="H53" s="180" t="s">
-        <v>43</v>
-      </c>
-      <c r="I53" s="180" t="s">
-        <v>33</v>
-      </c>
+        <v>162</v>
+      </c>
+      <c r="I53" s="180"/>
       <c r="J53" s="180" t="s">
         <v>46</v>
       </c>
-      <c r="K53" s="184">
-        <v>3</v>
-      </c>
+      <c r="K53" s="184"/>
       <c r="L53">
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:12" ht="280.5">
+    <row r="54" spans="1:12" ht="114.75">
       <c r="A54" s="89" t="s">
-        <v>21</v>
+        <v>135</v>
       </c>
       <c r="B54" s="89" t="s">
-        <v>371</v>
+        <v>376</v>
       </c>
       <c r="C54" s="89" t="s">
-        <v>372</v>
+        <v>377</v>
       </c>
       <c r="D54" s="182" t="s">
-        <v>373</v>
+        <v>378</v>
       </c>
       <c r="E54" s="183" t="s">
         <v>119</v>
       </c>
-      <c r="F54" s="89" t="s">
-        <v>236</v>
+      <c r="F54" s="182" t="s">
+        <v>453</v>
       </c>
       <c r="G54" s="89" t="s">
         <v>282</v>
       </c>
       <c r="H54" s="180" t="s">
+        <v>43</v>
+      </c>
+      <c r="I54" s="180" t="s">
+        <v>34</v>
+      </c>
+      <c r="J54" s="180" t="s">
+        <v>70</v>
+      </c>
+      <c r="K54" s="184">
+        <v>3</v>
+      </c>
+      <c r="L54">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" ht="222" customHeight="1">
+      <c r="A55" s="108" t="s">
+        <v>135</v>
+      </c>
+      <c r="B55" s="108" t="s">
+        <v>380</v>
+      </c>
+      <c r="C55" s="108" t="s">
+        <v>381</v>
+      </c>
+      <c r="D55" s="108" t="s">
+        <v>382</v>
+      </c>
+      <c r="E55" s="200" t="s">
+        <v>457</v>
+      </c>
+      <c r="F55" s="108" t="s">
+        <v>458</v>
+      </c>
+      <c r="G55" s="108" t="s">
+        <v>282</v>
+      </c>
+      <c r="H55" s="180" t="s">
         <v>162</v>
       </c>
-      <c r="I54" s="180"/>
-      <c r="J54" s="180" t="s">
-        <v>46</v>
-      </c>
-      <c r="K54" s="184"/>
-      <c r="L54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" ht="114.75">
-      <c r="A55" s="89" t="s">
-        <v>135</v>
-      </c>
-      <c r="B55" s="89" t="s">
-        <v>376</v>
-      </c>
-      <c r="C55" s="89" t="s">
-        <v>377</v>
-      </c>
-      <c r="D55" s="182" t="s">
-        <v>378</v>
-      </c>
-      <c r="E55" s="183" t="s">
-        <v>119</v>
-      </c>
-      <c r="F55" s="89" t="s">
-        <v>236</v>
-      </c>
-      <c r="G55" s="89" t="s">
-        <v>282</v>
-      </c>
-      <c r="H55" s="180" t="s">
-        <v>43</v>
-      </c>
       <c r="I55" s="180" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="J55" s="180" t="s">
         <v>70</v>
@@ -5370,21 +5558,21 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:12" ht="162" customHeight="1">
-      <c r="A56" s="108" t="s">
-        <v>135</v>
+    <row r="56" spans="1:12" ht="51">
+      <c r="A56" s="89" t="s">
+        <v>124</v>
       </c>
       <c r="B56" s="108" t="s">
-        <v>380</v>
-      </c>
-      <c r="C56" s="108" t="s">
-        <v>381</v>
-      </c>
-      <c r="D56" s="108" t="s">
-        <v>382</v>
-      </c>
+        <v>387</v>
+      </c>
+      <c r="C56" s="187" t="s">
+        <v>244</v>
+      </c>
+      <c r="D56" s="108"/>
       <c r="E56" s="108"/>
-      <c r="F56" s="108"/>
+      <c r="F56" s="182" t="s">
+        <v>453</v>
+      </c>
       <c r="G56" s="108" t="s">
         <v>282</v>
       </c>
@@ -5395,7 +5583,7 @@
         <v>33</v>
       </c>
       <c r="J56" s="180" t="s">
-        <v>70</v>
+        <v>46</v>
       </c>
       <c r="K56" s="184">
         <v>3</v>
@@ -5404,18 +5592,22 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:12" ht="45">
-      <c r="A57" s="89" t="s">
+    <row r="57" spans="1:12" ht="90">
+      <c r="A57" s="185" t="s">
         <v>124</v>
       </c>
-      <c r="B57" s="108" t="s">
-        <v>387</v>
-      </c>
-      <c r="C57" s="108"/>
-      <c r="D57" s="108"/>
-      <c r="E57" s="108"/>
-      <c r="F57" s="108"/>
-      <c r="G57" s="108" t="s">
+      <c r="B57" s="89" t="s">
+        <v>459</v>
+      </c>
+      <c r="C57" s="108" t="s">
+        <v>341</v>
+      </c>
+      <c r="D57" s="89"/>
+      <c r="E57" s="89"/>
+      <c r="F57" s="182" t="s">
+        <v>460</v>
+      </c>
+      <c r="G57" s="89" t="s">
         <v>282</v>
       </c>
       <c r="H57" s="180" t="s">
@@ -5427,34 +5619,38 @@
       <c r="J57" s="180" t="s">
         <v>46</v>
       </c>
-      <c r="K57" s="184">
-        <v>3</v>
-      </c>
+      <c r="K57" s="184"/>
       <c r="L57">
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:12" ht="90">
-      <c r="A58" s="185" t="s">
-        <v>124</v>
+    <row r="58" spans="1:12" ht="45">
+      <c r="A58" s="89" t="s">
+        <v>276</v>
       </c>
       <c r="B58" s="89" t="s">
-        <v>390</v>
+        <v>462</v>
       </c>
       <c r="C58" s="108" t="s">
         <v>244</v>
       </c>
-      <c r="D58" s="89"/>
-      <c r="E58" s="89"/>
-      <c r="F58" s="89"/>
+      <c r="D58" s="89" t="s">
+        <v>461</v>
+      </c>
+      <c r="E58" s="89" t="s">
+        <v>119</v>
+      </c>
+      <c r="F58" s="182" t="s">
+        <v>460</v>
+      </c>
       <c r="G58" s="89" t="s">
         <v>282</v>
       </c>
       <c r="H58" s="180" t="s">
-        <v>162</v>
+        <v>43</v>
       </c>
       <c r="I58" s="180" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="J58" s="180" t="s">
         <v>46</v>
@@ -5464,79 +5660,85 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:12" ht="30">
-      <c r="A59" s="185" t="s">
+    <row r="59" spans="1:12" ht="60">
+      <c r="A59" s="174" t="s">
         <v>124</v>
       </c>
-      <c r="B59" s="89" t="s">
-        <v>391</v>
-      </c>
-      <c r="C59" s="108" t="s">
+      <c r="B59" s="186" t="s">
+        <v>463</v>
+      </c>
+      <c r="C59" s="187" t="s">
         <v>244</v>
       </c>
-      <c r="D59" s="89"/>
-      <c r="E59" s="89"/>
-      <c r="F59" s="89"/>
-      <c r="G59" s="89" t="s">
+      <c r="D59" s="186"/>
+      <c r="E59" s="186"/>
+      <c r="F59" s="182" t="s">
+        <v>460</v>
+      </c>
+      <c r="G59" s="186" t="s">
         <v>282</v>
       </c>
-      <c r="H59" s="180" t="s">
+      <c r="H59" s="188" t="s">
         <v>43</v>
       </c>
-      <c r="I59" s="180" t="s">
+      <c r="I59" s="188" t="s">
         <v>45</v>
       </c>
-      <c r="J59" s="180" t="s">
+      <c r="J59" s="188" t="s">
         <v>46</v>
       </c>
-      <c r="K59" s="184"/>
+      <c r="K59" s="189"/>
       <c r="L59">
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:12" ht="60">
-      <c r="A60" s="174" t="s">
+    <row r="60" spans="1:12" ht="75">
+      <c r="A60" s="190" t="s">
         <v>124</v>
       </c>
-      <c r="B60" s="186" t="s">
-        <v>392</v>
-      </c>
-      <c r="C60" s="187" t="s">
+      <c r="B60" s="191" t="s">
+        <v>464</v>
+      </c>
+      <c r="C60" s="192" t="s">
         <v>244</v>
       </c>
-      <c r="D60" s="186"/>
-      <c r="E60" s="186"/>
-      <c r="F60" s="186"/>
-      <c r="G60" s="186" t="s">
-        <v>282</v>
-      </c>
-      <c r="H60" s="188" t="s">
-        <v>43</v>
-      </c>
-      <c r="I60" s="188" t="s">
-        <v>45</v>
-      </c>
-      <c r="J60" s="188" t="s">
-        <v>46</v>
-      </c>
-      <c r="K60" s="189"/>
+      <c r="D60" s="191"/>
+      <c r="E60" s="191"/>
+      <c r="F60" s="198" t="s">
+        <v>460</v>
+      </c>
+      <c r="G60" s="191" t="s">
+        <v>430</v>
+      </c>
+      <c r="H60" s="193" t="s">
+        <v>31</v>
+      </c>
+      <c r="I60" s="193" t="s">
+        <v>33</v>
+      </c>
+      <c r="J60" s="193" t="s">
+        <v>70</v>
+      </c>
+      <c r="K60" s="194"/>
       <c r="L60">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:12" ht="30">
-      <c r="A61" s="190" t="s">
+    <row r="61" spans="1:12" ht="45">
+      <c r="A61" s="185" t="s">
         <v>124</v>
       </c>
-      <c r="B61" s="191" t="s">
-        <v>394</v>
-      </c>
-      <c r="C61" s="192" t="s">
+      <c r="B61" s="76" t="s">
+        <v>465</v>
+      </c>
+      <c r="C61" s="195" t="s">
         <v>244</v>
       </c>
-      <c r="D61" s="191"/>
-      <c r="E61" s="191"/>
-      <c r="F61" s="191"/>
+      <c r="D61" s="76"/>
+      <c r="E61" s="76"/>
+      <c r="F61" s="198" t="s">
+        <v>460</v>
+      </c>
       <c r="G61" s="191" t="s">
         <v>430</v>
       </c>
@@ -5549,32 +5751,36 @@
       <c r="J61" s="193" t="s">
         <v>70</v>
       </c>
-      <c r="K61" s="194"/>
+      <c r="K61" s="196"/>
       <c r="L61">
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:12" ht="30">
-      <c r="A62" s="185" t="s">
-        <v>124</v>
+    <row r="62" spans="1:12" ht="45">
+      <c r="A62" s="197" t="s">
+        <v>276</v>
       </c>
       <c r="B62" s="76" t="s">
-        <v>396</v>
+        <v>398</v>
       </c>
       <c r="C62" s="195" t="s">
         <v>244</v>
       </c>
       <c r="D62" s="76"/>
-      <c r="E62" s="76"/>
-      <c r="F62" s="76"/>
+      <c r="E62" s="76" t="s">
+        <v>466</v>
+      </c>
+      <c r="F62" s="198" t="s">
+        <v>460</v>
+      </c>
       <c r="G62" s="191" t="s">
         <v>430</v>
       </c>
       <c r="H62" s="193" t="s">
-        <v>31</v>
+        <v>162</v>
       </c>
       <c r="I62" s="193" t="s">
-        <v>33</v>
+        <v>45</v>
       </c>
       <c r="J62" s="193" t="s">
         <v>70</v>
@@ -5584,19 +5790,23 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:12" ht="45">
-      <c r="A63" s="197" t="s">
-        <v>276</v>
+    <row r="63" spans="1:12" ht="65.25" customHeight="1">
+      <c r="A63" s="185" t="s">
+        <v>124</v>
       </c>
       <c r="B63" s="76" t="s">
-        <v>398</v>
+        <v>428</v>
       </c>
       <c r="C63" s="195" t="s">
         <v>244</v>
       </c>
       <c r="D63" s="76"/>
-      <c r="E63" s="76"/>
-      <c r="F63" s="76"/>
+      <c r="E63" s="76" t="s">
+        <v>25</v>
+      </c>
+      <c r="F63" s="198" t="s">
+        <v>467</v>
+      </c>
       <c r="G63" s="191" t="s">
         <v>430</v>
       </c>
@@ -5604,7 +5814,7 @@
         <v>162</v>
       </c>
       <c r="I63" s="193" t="s">
-        <v>45</v>
+        <v>34</v>
       </c>
       <c r="J63" s="193" t="s">
         <v>70</v>
@@ -5614,25 +5824,29 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:12" ht="65.25" customHeight="1">
+    <row r="64" spans="1:12" ht="60">
       <c r="A64" s="185" t="s">
         <v>124</v>
       </c>
       <c r="B64" s="76" t="s">
-        <v>428</v>
-      </c>
-      <c r="C64" s="195"/>
+        <v>468</v>
+      </c>
+      <c r="C64" s="195" t="s">
+        <v>244</v>
+      </c>
       <c r="D64" s="76"/>
       <c r="E64" s="76"/>
-      <c r="F64" s="76"/>
+      <c r="F64" s="198" t="s">
+        <v>460</v>
+      </c>
       <c r="G64" s="191" t="s">
         <v>430</v>
       </c>
       <c r="H64" s="193" t="s">
-        <v>162</v>
+        <v>43</v>
       </c>
       <c r="I64" s="193" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="J64" s="193" t="s">
         <v>70</v>
@@ -5642,78 +5856,27 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:12" ht="30">
-      <c r="A65" s="185" t="s">
-        <v>124</v>
-      </c>
-      <c r="B65" s="76" t="s">
-        <v>399</v>
-      </c>
-      <c r="C65" s="195" t="s">
-        <v>244</v>
-      </c>
-      <c r="D65" s="76"/>
-      <c r="E65" s="76"/>
-      <c r="F65" s="76"/>
-      <c r="G65" s="191" t="s">
-        <v>430</v>
-      </c>
-      <c r="H65" s="193" t="s">
-        <v>43</v>
-      </c>
-      <c r="I65" s="193" t="s">
-        <v>45</v>
-      </c>
-      <c r="J65" s="193" t="s">
-        <v>70</v>
-      </c>
-      <c r="K65" s="196"/>
-      <c r="L65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" ht="60">
-      <c r="A66" s="185" t="s">
-        <v>124</v>
-      </c>
-      <c r="B66" s="76" t="s">
-        <v>400</v>
-      </c>
-      <c r="C66" s="76" t="s">
-        <v>401</v>
-      </c>
-      <c r="D66" s="198"/>
-      <c r="E66" s="199"/>
-      <c r="F66" s="76" t="s">
-        <v>338</v>
-      </c>
-      <c r="G66" s="191" t="s">
-        <v>430</v>
-      </c>
-      <c r="H66" s="193" t="s">
-        <v>162</v>
-      </c>
-      <c r="I66" s="193" t="s">
-        <v>33</v>
-      </c>
-      <c r="J66" s="193" t="s">
-        <v>46</v>
-      </c>
-      <c r="K66" s="196"/>
-      <c r="L66">
-        <v>1</v>
-      </c>
-    </row>
   </sheetData>
-  <conditionalFormatting sqref="A2:A57">
-    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="achieved and ongoing">
+  <conditionalFormatting sqref="A2:A56">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="achieved and ongoing">
       <formula>NOT(ISERROR(SEARCH("achieved and ongoing",A2)))</formula>
     </cfRule>
-    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="underway">
+    <cfRule type="containsText" dxfId="10" priority="5" operator="containsText" text="underway">
       <formula>NOT(ISERROR(SEARCH("underway",A2)))</formula>
     </cfRule>
+    <cfRule type="containsText" dxfId="9" priority="6" operator="containsText" text="not started">
+      <formula>NOT(ISERROR(SEARCH("not started",A2)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A58">
+    <cfRule type="containsText" dxfId="8" priority="1" operator="containsText" text="achieved and ongoing">
+      <formula>NOT(ISERROR(SEARCH("achieved and ongoing",A58)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="7" priority="2" operator="containsText" text="underway">
+      <formula>NOT(ISERROR(SEARCH("underway",A58)))</formula>
+    </cfRule>
     <cfRule type="containsText" dxfId="6" priority="3" operator="containsText" text="not started">
-      <formula>NOT(ISERROR(SEARCH("not started",A2)))</formula>
+      <formula>NOT(ISERROR(SEARCH("not started",A58)))</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -12105,6 +12268,26 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <TaxCatchAll xmlns="12c1d019-452c-4f5f-9397-ffc6d392f7a1" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="689033e7-fc09-4c40-a3c6-00594cf9aea0">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x01010085C9F2CD37B1374EBC535C74F202A173" ma:contentTypeVersion="18" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="2790b99a3d72608f6269c6bfcacd7c1f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="689033e7-fc09-4c40-a3c6-00594cf9aea0" xmlns:ns3="12c1d019-452c-4f5f-9397-ffc6d392f7a1" xmlns:ns4="ab9ea86b-b30e-4b69-aa01-b771721c3aef" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="b3cc7b546f64d0c596c0b9fcf59ff446" ns2:_="" ns3:_="" ns4:_="">
     <xsd:import namespace="689033e7-fc09-4c40-a3c6-00594cf9aea0"/>
@@ -12358,27 +12541,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <TaxCatchAll xmlns="12c1d019-452c-4f5f-9397-ffc6d392f7a1" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="689033e7-fc09-4c40-a3c6-00594cf9aea0">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFA26091-165F-4BC2-8D88-D31BD362455C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CD9C593-6A79-4D85-9CD9-DE63E0BC27F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="12c1d019-452c-4f5f-9397-ffc6d392f7a1"/>
+    <ds:schemaRef ds:uri="689033e7-fc09-4c40-a3c6-00594cf9aea0"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1EC452F4-A49D-429D-AB97-7861B01AC740}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -12396,23 +12578,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5CD9C593-6A79-4D85-9CD9-DE63E0BC27F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="12c1d019-452c-4f5f-9397-ffc6d392f7a1"/>
-    <ds:schemaRef ds:uri="689033e7-fc09-4c40-a3c6-00594cf9aea0"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{EFA26091-165F-4BC2-8D88-D31BD362455C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>